<commit_message>
providing descriptive statistics in a new sheet Summary Statistics
</commit_message>
<xml_diff>
--- a/supermarket_sales.xlsx
+++ b/supermarket_sales.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analyst\Excel\Projects\Supermarket_Sales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE323B0-87C2-4C44-AF49-270B2F930959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BEC864-8CF6-4987-A939-C449B375565D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADA1FA73-857F-49C7-A2C4-BADC7F2D5686}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ADA1FA73-857F-49C7-A2C4-BADC7F2D5686}"/>
   </bookViews>
   <sheets>
     <sheet name="supermarket_sales" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary Statistics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7017" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7048" uniqueCount="1054">
   <si>
     <t>cogs</t>
   </si>
@@ -3139,6 +3140,60 @@
   </si>
   <si>
     <t>rating</t>
+  </si>
+  <si>
+    <t>total sales</t>
+  </si>
+  <si>
+    <t>average sales</t>
+  </si>
+  <si>
+    <t>median sales</t>
+  </si>
+  <si>
+    <t>sales range</t>
+  </si>
+  <si>
+    <t>max sales</t>
+  </si>
+  <si>
+    <t>min sales</t>
+  </si>
+  <si>
+    <t>sales std</t>
+  </si>
+  <si>
+    <t>sales data</t>
+  </si>
+  <si>
+    <t>total sales by branch</t>
+  </si>
+  <si>
+    <t>average sales by branch</t>
+  </si>
+  <si>
+    <t>sales by product line</t>
+  </si>
+  <si>
+    <t>average sales by product line</t>
+  </si>
+  <si>
+    <t>sales by customer type</t>
+  </si>
+  <si>
+    <t>average sales by customer type</t>
+  </si>
+  <si>
+    <t>sales by gender</t>
+  </si>
+  <si>
+    <t>average sales by gender</t>
+  </si>
+  <si>
+    <t>average rating</t>
+  </si>
+  <si>
+    <t>median rating</t>
   </si>
 </sst>
 </file>
@@ -3150,7 +3205,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3281,6 +3336,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3628,7 +3691,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -3637,6 +3700,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4073,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{168D3081-7B3F-4517-B5ED-17D53E725BDA}">
   <dimension ref="A1:Q1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="B975" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57157,4 +57223,314 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06658139-06A6-4592-AA6D-023C994BE37D}">
+  <dimension ref="B2:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38:B39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C2" s="9" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C3" s="3">
+        <f>SUM(sales[total])</f>
+        <v>322967.42999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C4" s="3">
+        <f>AVERAGE(sales[total])</f>
+        <v>322.96742999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="C5" s="3">
+        <f>MEDIAN(sales[total])</f>
+        <v>253.85000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C6" s="3">
+        <f>MAX(sales[total])</f>
+        <v>1042.6500000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C7" s="3">
+        <f>MIN(sales[total])</f>
+        <v>10.68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C8" s="3">
+        <f>C6-C7</f>
+        <v>1031.97</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C9" s="3">
+        <f>_xlfn.STDEV.P(sales[total])</f>
+        <v>245.76258303471505</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12" s="9" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <f>SUMIF(sales[branch],'Summary Statistics'!B13,sales[total])</f>
+        <v>106200.57</v>
+      </c>
+      <c r="D13" s="3">
+        <f>AVERAGEIF(sales[branch],'Summary Statistics'!B13,sales[total])</f>
+        <v>312.35461764705883</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SUMIF(sales[branch],'Summary Statistics'!B14,sales[total])</f>
+        <v>106198.00000000006</v>
+      </c>
+      <c r="D14" s="3">
+        <f>AVERAGEIF(sales[branch],'Summary Statistics'!B14,sales[total])</f>
+        <v>319.87349397590378</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3">
+        <f>SUMIF(sales[branch],'Summary Statistics'!B15,sales[total])</f>
+        <v>110568.85999999994</v>
+      </c>
+      <c r="D15" s="3">
+        <f>AVERAGEIF(sales[branch],'Summary Statistics'!B15,sales[total])</f>
+        <v>337.10018292682912</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C18" s="9" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B19,sales[total])</f>
+        <v>49193.840000000018</v>
+      </c>
+      <c r="D19" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B19,sales[total])</f>
+        <v>323.64368421052643</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B20,sales[total])</f>
+        <v>54337.640000000007</v>
+      </c>
+      <c r="D20" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B20,sales[total])</f>
+        <v>319.6331764705883</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B21,sales[total])</f>
+        <v>53861.960000000028</v>
+      </c>
+      <c r="D21" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B21,sales[total])</f>
+        <v>336.63725000000017</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B22,sales[total])</f>
+        <v>55123.000000000007</v>
+      </c>
+      <c r="D22" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B22,sales[total])</f>
+        <v>332.06626506024099</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B23,sales[total])</f>
+        <v>56144.960000000014</v>
+      </c>
+      <c r="D23" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B23,sales[total])</f>
+        <v>322.67218390804607</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="3">
+        <f>SUMIF(sales[product line],'Summary Statistics'!B24,sales[total])</f>
+        <v>54306.030000000006</v>
+      </c>
+      <c r="D24" s="3">
+        <f>AVERAGEIF(sales[product line],'Summary Statistics'!B24,sales[total])</f>
+        <v>305.09005617977533</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C27" s="9" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3">
+        <f>SUMIF(sales[customer type],'Summary Statistics'!B28,sales[total])</f>
+        <v>164223.80999999985</v>
+      </c>
+      <c r="D28" s="3">
+        <f>AVERAGEIF(sales[customer type],'Summary Statistics'!B28,sales[total])</f>
+        <v>327.79203592814343</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="3">
+        <f>SUMIF(sales[customer type],'Summary Statistics'!B29,sales[total])</f>
+        <v>158743.61999999985</v>
+      </c>
+      <c r="D29" s="3">
+        <f>AVERAGEIF(sales[customer type],'Summary Statistics'!B29,sales[total])</f>
+        <v>318.12348697394759</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="32" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C32" s="9" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C33" s="3">
+        <f>SUMIF(sales[gender],'Summary Statistics'!B33,sales[total])</f>
+        <v>155084.16999999981</v>
+      </c>
+      <c r="D33" s="3">
+        <f>AVERAGEIF(sales[gender],'Summary Statistics'!B33,sales[total])</f>
+        <v>310.78991983967899</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3">
+        <f>SUMIF(sales[gender],'Summary Statistics'!B34,sales[total])</f>
+        <v>167883.25999999995</v>
+      </c>
+      <c r="D34" s="3">
+        <f>AVERAGEIF(sales[gender],'Summary Statistics'!B34,sales[total])</f>
+        <v>335.09632734530931</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="8" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C38" s="10">
+        <f>AVERAGE(sales[rating])</f>
+        <v>6.9727000000000032</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="8" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C39" s="10">
+        <f>MEDIAN(sales[rating])</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>